<commit_message>
added us 07 and 08
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerry\Documents\School\CS555\project\cs555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3046E25C-96F1-4B99-B9E0-A61944A5E2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C123EED-F285-44ED-AF00-ED3BEA8B05B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{E948F438-0122-49D3-838A-1AA98BDF6037}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{E948F438-0122-49D3-838A-1AA98BDF6037}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="2" r:id="rId1"/>
@@ -3739,7 +3739,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3965,8 +3965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C9483B-7C01-4C77-A27D-CBB71DE53C8D}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4230,7 +4230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180101A1-B95D-45DC-A1F9-B5ECF4BF83E7}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
us15,23,24,25 don, report updated
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\2022 Fall\CS 555\cs555\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202DAB44-6A8B-4A02-BB99-00753F8FDE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82D34EF-DB35-44DB-8B34-032B58E388E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-144" yWindow="312" windowWidth="31008" windowHeight="17112" activeTab="6" xr2:uid="{E948F438-0122-49D3-838A-1AA98BDF6037}"/>
+    <workbookView xWindow="-144" yWindow="312" windowWidth="31008" windowHeight="17112" activeTab="8" xr2:uid="{E948F438-0122-49D3-838A-1AA98BDF6037}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="2" r:id="rId1"/>
@@ -20,10 +20,11 @@
     <sheet name="Sprint 1" sheetId="3" r:id="rId5"/>
     <sheet name="Sprint 2" sheetId="8" r:id="rId6"/>
     <sheet name="Sprint 3" sheetId="9" r:id="rId7"/>
-    <sheet name="Stories" sheetId="7" r:id="rId8"/>
+    <sheet name="Sprint 4" sheetId="10" r:id="rId8"/>
+    <sheet name="Stories" sheetId="7" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="192">
   <si>
     <t>Initials</t>
   </si>
@@ -616,6 +617,12 @@
   </si>
   <si>
     <t>Birth after marriage of parents</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>On pace to complete user stories</t>
   </si>
 </sst>
 </file>
@@ -745,7 +752,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -788,6 +795,7 @@
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1182,10 +1190,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Burndown!$A$2:$A$5</c:f>
+              <c:f>Burndown!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>m/d</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>44830</c:v>
                 </c:pt>
@@ -1198,25 +1206,31 @@
                 <c:pt idx="3">
                   <c:v>44851</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>44865</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Burndown!$B$2:$B$5</c:f>
+              <c:f>Burndown!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -3056,9 +3070,9 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -3153,13 +3167,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5089F6BA-D448-47B4-AE24-DF66C8EF4E69}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -3396,7 +3410,9 @@
       <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
@@ -3411,6 +3427,9 @@
       <c r="D15" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="E15" s="4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
@@ -3425,8 +3444,11 @@
       <c r="D16" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>3</v>
       </c>
@@ -3439,8 +3461,11 @@
       <c r="D17" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>3</v>
       </c>
@@ -3453,8 +3478,11 @@
       <c r="D18" s="4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>3</v>
       </c>
@@ -3467,8 +3495,11 @@
       <c r="D19" s="4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>4</v>
       </c>
@@ -3482,7 +3513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>4</v>
       </c>
@@ -3496,7 +3527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>4</v>
       </c>
@@ -3510,7 +3541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>4</v>
       </c>
@@ -3524,7 +3555,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>4</v>
       </c>
@@ -3538,7 +3569,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>4</v>
       </c>
@@ -3897,15 +3928,15 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -3937,7 +3968,7 @@
         <v>44830</v>
       </c>
       <c r="B2" s="4">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C2">
         <v>6</v>
@@ -3952,7 +3983,7 @@
         <v>44837</v>
       </c>
       <c r="B3" s="4">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C3" s="4">
         <f>B2-B3</f>
@@ -3974,7 +4005,7 @@
         <v>44844</v>
       </c>
       <c r="B4">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C4" s="4">
         <f t="shared" ref="C4:C5" si="0">B3-B4</f>
@@ -3990,7 +4021,7 @@
         <v>44851</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C5" s="4">
         <f t="shared" si="0"/>
@@ -4002,7 +4033,18 @@
       <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="8">
+        <v>44865</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>250</v>
+      </c>
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -4124,18 +4166,18 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4349,6 +4391,9 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
+      <c r="B15" s="26" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -4386,19 +4431,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180101A1-B95D-45DC-A1F9-B5ECF4BF83E7}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4611,7 +4656,9 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="24"/>
+      <c r="B10" s="26" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" s="24" t="s">
@@ -4619,7 +4666,9 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="25"/>
+      <c r="B12" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="25"/>
@@ -4633,6 +4682,16 @@
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="24" t="s">
         <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -4642,20 +4701,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A728D4E-6196-47CF-B7F5-353323ADCD08}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="26.77734375" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4699,13 +4758,22 @@
         <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>57</v>
+        <v>188</v>
       </c>
       <c r="E2">
         <v>25</v>
       </c>
       <c r="F2">
         <v>120</v>
+      </c>
+      <c r="G2">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>300</v>
+      </c>
+      <c r="I2" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -4719,13 +4787,22 @@
         <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>57</v>
+        <v>188</v>
       </c>
       <c r="E3">
         <v>25</v>
       </c>
       <c r="F3">
         <v>120</v>
+      </c>
+      <c r="G3">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>300</v>
+      </c>
+      <c r="I3" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -4739,13 +4816,22 @@
         <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>57</v>
+        <v>188</v>
       </c>
       <c r="E4">
         <v>25</v>
       </c>
       <c r="F4">
         <v>120</v>
+      </c>
+      <c r="G4">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>300</v>
+      </c>
+      <c r="I4" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -4759,13 +4845,22 @@
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>57</v>
+        <v>188</v>
       </c>
       <c r="E5">
         <v>25</v>
       </c>
       <c r="F5">
         <v>120</v>
+      </c>
+      <c r="G5">
+        <v>25</v>
+      </c>
+      <c r="H5">
+        <v>300</v>
+      </c>
+      <c r="I5" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -4779,13 +4874,22 @@
         <v>175</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>57</v>
+        <v>188</v>
       </c>
       <c r="E6">
         <v>25</v>
       </c>
       <c r="F6">
         <v>120</v>
+      </c>
+      <c r="G6">
+        <v>25</v>
+      </c>
+      <c r="H6">
+        <v>300</v>
+      </c>
+      <c r="I6" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -4799,7 +4903,7 @@
         <v>175</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>57</v>
+        <v>188</v>
       </c>
       <c r="E7">
         <v>25</v>
@@ -4807,27 +4911,270 @@
       <c r="F7">
         <v>120</v>
       </c>
+      <c r="G7">
+        <v>25</v>
+      </c>
+      <c r="H7">
+        <v>300</v>
+      </c>
+      <c r="I7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="24" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="25"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="25"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="25"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="24" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>182</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83123682-8ED9-433A-8356-FCAF37546C7B}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2">
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <v>120</v>
+      </c>
+      <c r="I2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>120</v>
+      </c>
+      <c r="I3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>120</v>
+      </c>
+      <c r="I4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>120</v>
+      </c>
+      <c r="I5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6">
+        <v>25</v>
+      </c>
+      <c r="F6">
+        <v>120</v>
+      </c>
+      <c r="I6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7">
+        <v>25</v>
+      </c>
+      <c r="F7">
+        <v>120</v>
+      </c>
+      <c r="I7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADC1019-8BDC-4EF6-9036-A457273E0BB7}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.21875" style="15" customWidth="1"/>
-    <col min="2" max="2" width="32.21875" style="15" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" style="15" customWidth="1"/>
     <col min="3" max="3" width="95" style="15" customWidth="1"/>
-    <col min="4" max="26" width="12.21875" style="15" customWidth="1"/>
+    <col min="4" max="26" width="12.109375" style="15" customWidth="1"/>
     <col min="27" max="16384" width="16.44140625" style="15"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
turned numbers file into excel spreadsheet file
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndCh\Documents\Coding Projects\cs555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B15074-145E-4787-8D44-F437BDB02B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9684B2-A571-42EB-8007-418772809B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{E948F438-0122-49D3-838A-1AA98BDF6037}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{E948F438-0122-49D3-838A-1AA98BDF6037}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="193">
   <si>
     <t>Initials</t>
   </si>
@@ -218,9 +218,6 @@
   </si>
   <si>
     <t>Completed</t>
-  </si>
-  <si>
-    <t>pending</t>
   </si>
   <si>
     <t>Keep Doing:</t>
@@ -3071,27 +3068,27 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" t="s">
         <v>175</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>176</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" t="s">
         <v>178</v>
-      </c>
-      <c r="E4" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -3150,7 +3147,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -3167,7 +3164,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -3184,7 +3181,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -3201,7 +3198,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -3215,10 +3212,10 @@
         <v>29</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -3232,10 +3229,10 @@
         <v>31</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -3252,7 +3249,7 @@
         <v>9</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -3269,7 +3266,7 @@
         <v>9</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -3286,7 +3283,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -3303,7 +3300,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -3317,10 +3314,10 @@
         <v>41</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -3334,10 +3331,10 @@
         <v>43</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -3354,7 +3351,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -3371,7 +3368,7 @@
         <v>9</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -3388,7 +3385,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -3405,7 +3402,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -3413,16 +3410,16 @@
         <v>3</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>134</v>
-      </c>
       <c r="D18" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -3430,16 +3427,16 @@
         <v>3</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>137</v>
-      </c>
       <c r="D19" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -3447,10 +3444,10 @@
         <v>4</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>143</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>9</v>
@@ -3461,10 +3458,10 @@
         <v>4</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>146</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>9</v>
@@ -3475,10 +3472,10 @@
         <v>4</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>6</v>
@@ -3489,10 +3486,10 @@
         <v>4</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>155</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>6</v>
@@ -3503,13 +3500,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>161</v>
-      </c>
       <c r="D24" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -3517,13 +3514,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>164</v>
-      </c>
       <c r="D25" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3543,19 +3540,19 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F3" s="9"/>
     </row>
@@ -3565,13 +3562,13 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F6" s="9"/>
     </row>
@@ -3581,7 +3578,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F8" s="9"/>
     </row>
@@ -3610,22 +3607,22 @@
         <v>15</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -3638,7 +3635,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="12">
         <v>42527</v>
@@ -3654,7 +3651,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="12">
         <v>42540</v>
@@ -3679,7 +3676,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="12">
         <v>42554</v>
@@ -3704,7 +3701,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" s="12">
         <v>42568</v>
@@ -3729,7 +3726,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="12">
         <v>42582</v>
@@ -3884,22 +3881,22 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -4175,7 +4172,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E2">
         <v>25</v>
@@ -4190,7 +4187,7 @@
         <v>300</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -4204,7 +4201,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E3">
         <v>25</v>
@@ -4219,7 +4216,7 @@
         <v>300</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -4233,7 +4230,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E4">
         <v>25</v>
@@ -4248,7 +4245,7 @@
         <v>300</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -4262,7 +4259,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E5">
         <v>25</v>
@@ -4277,7 +4274,7 @@
         <v>300</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -4288,10 +4285,10 @@
         <v>29</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E6">
         <v>25</v>
@@ -4306,7 +4303,7 @@
         <v>300</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -4317,10 +4314,10 @@
         <v>31</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E7">
         <v>25</v>
@@ -4335,29 +4332,29 @@
         <v>300</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -4365,17 +4362,17 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -4441,7 +4438,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E2">
         <v>25</v>
@@ -4456,7 +4453,7 @@
         <v>300</v>
       </c>
       <c r="I2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -4464,13 +4461,13 @@
         <v>34</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E3">
         <v>25</v>
@@ -4485,7 +4482,7 @@
         <v>300</v>
       </c>
       <c r="I3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -4499,7 +4496,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E4">
         <v>25</v>
@@ -4514,7 +4511,7 @@
         <v>300</v>
       </c>
       <c r="I4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -4528,7 +4525,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E5">
         <v>25</v>
@@ -4543,7 +4540,7 @@
         <v>300</v>
       </c>
       <c r="I5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -4554,10 +4551,10 @@
         <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E6">
         <v>25</v>
@@ -4572,7 +4569,7 @@
         <v>300</v>
       </c>
       <c r="I6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -4583,10 +4580,10 @@
         <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E7">
         <v>25</v>
@@ -4601,27 +4598,27 @@
         <v>300</v>
       </c>
       <c r="I7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -4635,17 +4632,17 @@
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -4712,7 +4709,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E2">
         <v>25</v>
@@ -4727,7 +4724,7 @@
         <v>300</v>
       </c>
       <c r="I2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -4741,7 +4738,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E3">
         <v>25</v>
@@ -4756,7 +4753,7 @@
         <v>300</v>
       </c>
       <c r="I3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -4770,7 +4767,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E4">
         <v>25</v>
@@ -4785,7 +4782,7 @@
         <v>300</v>
       </c>
       <c r="I4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -4799,7 +4796,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E5">
         <v>25</v>
@@ -4814,21 +4811,21 @@
         <v>300</v>
       </c>
       <c r="I5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>134</v>
-      </c>
       <c r="C6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E6">
         <v>25</v>
@@ -4843,21 +4840,21 @@
         <v>300</v>
       </c>
       <c r="I6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>137</v>
-      </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E7">
         <v>25</v>
@@ -4872,27 +4869,27 @@
         <v>300</v>
       </c>
       <c r="I7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -4906,17 +4903,17 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -4930,8 +4927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83123682-8ED9-433A-8356-FCAF37546C7B}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4974,16 +4971,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E2">
         <v>25</v>
@@ -4998,21 +4995,21 @@
         <v>300</v>
       </c>
       <c r="I2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E3">
         <v>25</v>
@@ -5027,21 +5024,21 @@
         <v>300</v>
       </c>
       <c r="I3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>106</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>107</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E4">
         <v>25</v>
@@ -5056,21 +5053,21 @@
         <v>300</v>
       </c>
       <c r="I4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E5">
         <v>25</v>
@@ -5085,21 +5082,21 @@
         <v>300</v>
       </c>
       <c r="I5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>113</v>
-      </c>
       <c r="C6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>57</v>
+        <v>187</v>
       </c>
       <c r="E6">
         <v>25</v>
@@ -5107,22 +5104,28 @@
       <c r="F6">
         <v>120</v>
       </c>
+      <c r="G6">
+        <v>25</v>
+      </c>
+      <c r="H6">
+        <v>300</v>
+      </c>
       <c r="I6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>116</v>
-      </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>57</v>
+        <v>187</v>
       </c>
       <c r="E7">
         <v>25</v>
@@ -5130,8 +5133,14 @@
       <c r="F7">
         <v>120</v>
       </c>
+      <c r="G7">
+        <v>25</v>
+      </c>
+      <c r="H7">
+        <v>300</v>
+      </c>
       <c r="I7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -5143,7 +5152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADC1019-8BDC-4EF6-9036-A457273E0BB7}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
@@ -5164,7 +5173,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
@@ -5198,7 +5207,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5209,7 +5218,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5220,7 +5229,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5231,7 +5240,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5242,7 +5251,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5253,7 +5262,7 @@
         <v>31</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5264,7 +5273,7 @@
         <v>33</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5272,10 +5281,10 @@
         <v>34</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5286,7 +5295,7 @@
         <v>37</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5297,29 +5306,29 @@
         <v>39</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>92</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="C13" s="17" t="s">
         <v>95</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5330,7 +5339,7 @@
         <v>41</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5341,7 +5350,7 @@
         <v>43</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5352,84 +5361,84 @@
         <v>45</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B17" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>155</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>152</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="C19" s="17" t="s">
         <v>107</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>173</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="C21" s="17" t="s">
         <v>113</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="C22" s="17" t="s">
         <v>116</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="C23" s="17" t="s">
         <v>119</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5440,7 +5449,7 @@
         <v>47</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5451,7 +5460,7 @@
         <v>49</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5462,194 +5471,194 @@
         <v>51</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="C27" s="17" t="s">
         <v>125</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="C28" s="17" t="s">
         <v>128</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="C29" s="17" t="s">
         <v>131</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B30" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="C30" s="17" t="s">
         <v>134</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="C31" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="C32" s="17" t="s">
         <v>140</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="C33" s="17" t="s">
         <v>143</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B34" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="C34" s="17" t="s">
         <v>146</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="C35" s="17" t="s">
         <v>149</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B36" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="17" t="s">
         <v>104</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B37" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="17" t="s">
         <v>101</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="B38" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="C38" s="17" t="s">
         <v>158</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B39" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="C39" s="17" t="s">
         <v>161</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="B40" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="C40" s="17" t="s">
         <v>164</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="B41" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="B41" s="18" t="s">
+      <c r="C41" s="17" t="s">
         <v>167</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B42" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="B42" s="18" t="s">
+      <c r="C42" s="17" t="s">
         <v>170</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B43" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="17" t="s">
         <v>110</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>